<commit_message>
Ultimos cambios en Temisco
</commit_message>
<xml_diff>
--- a/campos_info/weibull_resumen.xlsx
+++ b/campos_info/weibull_resumen.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16500" tabRatio="500"/>
+    <workbookView xWindow="940" yWindow="0" windowWidth="25600" windowHeight="16500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
+    <sheet name="Anuales" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -597,7 +598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:G1"/>
     </sheetView>
   </sheetViews>
@@ -2744,4 +2745,1184 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C1">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D1">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E1">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="F1">
+        <v>1.9084364924755301E-3</v>
+      </c>
+      <c r="G1">
+        <v>1.97801325374013</v>
+      </c>
+      <c r="H1">
+        <v>0.319279253862434</v>
+      </c>
+      <c r="I1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="F2">
+        <v>4.14399041389197E-4</v>
+      </c>
+      <c r="G2">
+        <v>1.3842632546911899</v>
+      </c>
+      <c r="H2">
+        <v>8.8271214249260904E-2</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1.5E-3</v>
+      </c>
+      <c r="C3">
+        <v>1.5E-3</v>
+      </c>
+      <c r="D3">
+        <v>1.5E-3</v>
+      </c>
+      <c r="E3">
+        <v>1.5E-3</v>
+      </c>
+      <c r="F3">
+        <v>5.6756361826644898E-3</v>
+      </c>
+      <c r="G3">
+        <v>1.9772372100951101</v>
+      </c>
+      <c r="H3">
+        <v>0.366250800748393</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>1.5E-3</v>
+      </c>
+      <c r="C4">
+        <v>1.5E-3</v>
+      </c>
+      <c r="D4">
+        <v>1.5E-3</v>
+      </c>
+      <c r="E4">
+        <v>1.5E-3</v>
+      </c>
+      <c r="F4">
+        <v>1.2378691610517099E-3</v>
+      </c>
+      <c r="G4">
+        <v>1.38562017648697</v>
+      </c>
+      <c r="H4">
+        <v>2.29904917085277E-2</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="C5">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="D5">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="E5">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="F5">
+        <v>9.5079668990434903E-3</v>
+      </c>
+      <c r="G5">
+        <v>1.9731193499691599</v>
+      </c>
+      <c r="H5">
+        <v>0.20442020318512</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="C6">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="D6">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="E6">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="F6">
+        <v>2.03156968801929E-3</v>
+      </c>
+      <c r="G6">
+        <v>1.3928722702365399</v>
+      </c>
+      <c r="H6">
+        <v>5.5151382390454001E-2</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F7">
+        <v>1.89463919050324E-2</v>
+      </c>
+      <c r="G7">
+        <v>2.0431532253482301</v>
+      </c>
+      <c r="H7">
+        <v>0.23035020519579399</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F8">
+        <v>3.9856211393866801E-3</v>
+      </c>
+      <c r="G8">
+        <v>1.3298664082140901</v>
+      </c>
+      <c r="H8">
+        <v>8.7411678396951201E-3</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>1E-3</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1.69583340781817E-3</v>
+      </c>
+      <c r="G9">
+        <v>1.2345137935638399</v>
+      </c>
+      <c r="H9">
+        <v>3.9549073674308703E-2</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>1E-3</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>2.5765840575334701E-4</v>
+      </c>
+      <c r="G10">
+        <v>0.96475386948401798</v>
+      </c>
+      <c r="H10">
+        <v>7.7338772307235501E-2</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>4.3633986287244103E-3</v>
+      </c>
+      <c r="G11">
+        <v>1.23780460980101</v>
+      </c>
+      <c r="H11">
+        <v>7.6267822984057404E-2</v>
+      </c>
+      <c r="I11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>6.7628329423236099E-4</v>
+      </c>
+      <c r="G12">
+        <v>0.940123483915974</v>
+      </c>
+      <c r="H12">
+        <v>0.12536843791367899</v>
+      </c>
+      <c r="I12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>8.1280100393522695E-3</v>
+      </c>
+      <c r="G13">
+        <v>1.2842206120036499</v>
+      </c>
+      <c r="H13">
+        <v>0.42925004171654102</v>
+      </c>
+      <c r="I13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>1.24963585769882E-3</v>
+      </c>
+      <c r="G14">
+        <v>0.98732501405636897</v>
+      </c>
+      <c r="H14">
+        <v>0.20326390318162499</v>
+      </c>
+      <c r="I14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>0.01</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>1.5971900222063899E-2</v>
+      </c>
+      <c r="G15">
+        <v>1.2855219107692899</v>
+      </c>
+      <c r="H15">
+        <v>0.18817094875634399</v>
+      </c>
+      <c r="I15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>0.01</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>2.4719067362624502E-3</v>
+      </c>
+      <c r="G16">
+        <v>0.95553050297585196</v>
+      </c>
+      <c r="H16">
+        <v>5.8433574616541299E-2</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>1E-3</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>1.3555548185636001E-3</v>
+      </c>
+      <c r="G17">
+        <v>1.2552323978250599</v>
+      </c>
+      <c r="H17">
+        <v>0.13811872675374001</v>
+      </c>
+      <c r="I17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>1E-3</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>3.6505803855203502E-4</v>
+      </c>
+      <c r="G18">
+        <v>1.09157700417993</v>
+      </c>
+      <c r="H18">
+        <v>0.495432386846555</v>
+      </c>
+      <c r="I18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>4.12467851868413E-3</v>
+      </c>
+      <c r="G19">
+        <v>1.28392029356869</v>
+      </c>
+      <c r="H19">
+        <v>0.20021213639145299</v>
+      </c>
+      <c r="I19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>1.1015811990259599E-3</v>
+      </c>
+      <c r="G20">
+        <v>1.1354257523743101</v>
+      </c>
+      <c r="H20">
+        <v>0.380051944209082</v>
+      </c>
+      <c r="I20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>6.5513833329157601E-3</v>
+      </c>
+      <c r="G21">
+        <v>1.1509094070683099</v>
+      </c>
+      <c r="H21">
+        <v>0.482321477719867</v>
+      </c>
+      <c r="I21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>1.74711534527732E-3</v>
+      </c>
+      <c r="G22">
+        <v>1.0361747532329399</v>
+      </c>
+      <c r="H22">
+        <v>0.72770226072784405</v>
+      </c>
+      <c r="I22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0.01</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>1.24209187495645E-2</v>
+      </c>
+      <c r="G23">
+        <v>1.1541186370910399</v>
+      </c>
+      <c r="H23">
+        <v>0.366928762999845</v>
+      </c>
+      <c r="I23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0.01</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>3.3132711200353601E-3</v>
+      </c>
+      <c r="G24">
+        <v>1.0316779911865599</v>
+      </c>
+      <c r="H24">
+        <v>0.471135948194289</v>
+      </c>
+      <c r="I24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>1E-3</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>2.2517644538677202E-3</v>
+      </c>
+      <c r="G25">
+        <v>1.81194000118803</v>
+      </c>
+      <c r="H25">
+        <v>0.377292951717138</v>
+      </c>
+      <c r="I25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>1E-3</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>4.5023484835890801E-4</v>
+      </c>
+      <c r="G26">
+        <v>1.29078503723055</v>
+      </c>
+      <c r="H26">
+        <v>7.6069782355433196E-3</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>6.4459294822511396E-3</v>
+      </c>
+      <c r="G27">
+        <v>1.7891098062373201</v>
+      </c>
+      <c r="H27">
+        <v>0.11681436023526801</v>
+      </c>
+      <c r="I27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>1.2960439289970301E-3</v>
+      </c>
+      <c r="G28">
+        <v>1.29906901631668</v>
+      </c>
+      <c r="H28">
+        <v>5.3023789899728502E-2</v>
+      </c>
+      <c r="I28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>1.0761387644495799E-2</v>
+      </c>
+      <c r="G29">
+        <v>1.82876966438887</v>
+      </c>
+      <c r="H29">
+        <v>0.184027563233399</v>
+      </c>
+      <c r="I29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>2.1809825231056401E-3</v>
+      </c>
+      <c r="G30">
+        <v>1.33682208515547</v>
+      </c>
+      <c r="H30">
+        <v>0.13084481263937101</v>
+      </c>
+      <c r="I30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0.01</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>2.1233137800906798E-2</v>
+      </c>
+      <c r="G31">
+        <v>1.8227401471585201</v>
+      </c>
+      <c r="H31">
+        <v>0.26109540051616298</v>
+      </c>
+      <c r="I31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0.01</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>4.4626330059494897E-3</v>
+      </c>
+      <c r="G32">
+        <v>1.28362101218998</v>
+      </c>
+      <c r="H32">
+        <v>0.15128428418746501</v>
+      </c>
+      <c r="I32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>1E-3</v>
+      </c>
+      <c r="F33">
+        <v>1.6116871624178399E-3</v>
+      </c>
+      <c r="G33">
+        <v>1.3119586405747801</v>
+      </c>
+      <c r="H33">
+        <v>0.13780480254199401</v>
+      </c>
+      <c r="I33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34">
+        <v>0</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>1E-3</v>
+      </c>
+      <c r="F34">
+        <v>3.3237147030305901E-4</v>
+      </c>
+      <c r="G34">
+        <v>0.99347207762484702</v>
+      </c>
+      <c r="H34">
+        <v>0.37435124325101798</v>
+      </c>
+      <c r="I34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35">
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F35">
+        <v>4.9606787971784704E-3</v>
+      </c>
+      <c r="G35">
+        <v>1.2080574104197199</v>
+      </c>
+      <c r="H35">
+        <v>0.28646741346771398</v>
+      </c>
+      <c r="I35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36">
+        <v>0</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F36">
+        <v>1.0233365530762E-3</v>
+      </c>
+      <c r="G36">
+        <v>0.92773271840362403</v>
+      </c>
+      <c r="H36">
+        <v>0.465696365531371</v>
+      </c>
+      <c r="I36">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37">
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F37">
+        <v>8.5055842915500099E-3</v>
+      </c>
+      <c r="G37">
+        <v>1.3039083327249099</v>
+      </c>
+      <c r="H37">
+        <v>0.19240098971160299</v>
+      </c>
+      <c r="I37">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38">
+        <v>0</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F38">
+        <v>1.7711685868725801E-3</v>
+      </c>
+      <c r="G38">
+        <v>0.97716675006880604</v>
+      </c>
+      <c r="H38">
+        <v>9.3675515967147002E-2</v>
+      </c>
+      <c r="I38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39">
+        <v>0</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0.01</v>
+      </c>
+      <c r="F39">
+        <v>1.6804709817280598E-2</v>
+      </c>
+      <c r="G39">
+        <v>1.2639282717301601</v>
+      </c>
+      <c r="H39">
+        <v>0.18995161231087199</v>
+      </c>
+      <c r="I39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40">
+        <v>0</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0.01</v>
+      </c>
+      <c r="F40">
+        <v>3.5202625921716799E-3</v>
+      </c>
+      <c r="G40">
+        <v>0.95105048190653696</v>
+      </c>
+      <c r="H40">
+        <v>0.454305213235139</v>
+      </c>
+      <c r="I40">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>